<commit_message>
Pooh Points: normal 20260210
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-10.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-10.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V33"/>
+  <dimension ref="A1:V39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
     <col width="26" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="9" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
@@ -597,53 +597,53 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H2" t="n">
+        <v>15</v>
+      </c>
+      <c r="I2" t="n">
+        <v>13</v>
+      </c>
+      <c r="J2" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>2</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2</v>
+      </c>
+      <c r="P2" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>5</v>
+      </c>
+      <c r="R2" t="n">
+        <v>9</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>3</v>
+      </c>
+      <c r="V2" t="n">
         <v>4</v>
-      </c>
-      <c r="I2" t="n">
-        <v>4</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>2</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>2</v>
-      </c>
-      <c r="P2" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>2</v>
-      </c>
-      <c r="R2" t="n">
-        <v>6</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -679,41 +679,41 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>-2</v>
+        <v>7</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J3" t="n">
+        <v>7</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
         <v>4</v>
       </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q3" t="n">
         <v>3</v>
       </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>19</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
       <c r="R3" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -722,10 +722,10 @@
         <v>1</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V3" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -843,53 +843,53 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I5" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J5" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M5" t="n">
+        <v>5</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
         <v>4</v>
       </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>2</v>
-      </c>
       <c r="P5" t="n">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="Q5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R5" t="n">
+        <v>8</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
+        <v>4</v>
+      </c>
+      <c r="U5" t="n">
         <v>5</v>
       </c>
-      <c r="S5" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" t="n">
-        <v>3</v>
-      </c>
-      <c r="U5" t="n">
-        <v>2</v>
-      </c>
       <c r="V5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -910,17 +910,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>KeShawn Murphy</t>
+          <t>Meleek Thomas</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>AUB</t>
+          <t>ARK</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>VAN@AUB</t>
+          <t>ARK@LSU</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -929,49 +929,49 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I6" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J6" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>3</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q6" t="n">
         <v>6</v>
       </c>
-      <c r="K6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>2</v>
-      </c>
-      <c r="N6" t="n">
-        <v>2</v>
-      </c>
-      <c r="O6" t="n">
+      <c r="R6" t="n">
+        <v>13</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" t="n">
         <v>4</v>
       </c>
-      <c r="P6" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>3</v>
-      </c>
-      <c r="R6" t="n">
-        <v>5</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
       <c r="U6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V6" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -992,68 +992,68 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Meleek Thomas</t>
+          <t>KeShawn Murphy</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ARK</t>
+          <t>AUB</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ARK@LSU</t>
+          <t>VAN@AUB</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I7" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J7" t="n">
+        <v>6</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2</v>
+      </c>
+      <c r="O7" t="n">
+        <v>4</v>
+      </c>
+      <c r="P7" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q7" t="n">
         <v>3</v>
       </c>
-      <c r="K7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" t="n">
-        <v>2</v>
-      </c>
-      <c r="M7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>25</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>4</v>
-      </c>
       <c r="R7" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="V7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -1253,23 +1253,23 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I10" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -1281,25 +1281,25 @@
         <v>3</v>
       </c>
       <c r="P10" t="n">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="Q10" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R10" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="S10" t="n">
         <v>1</v>
       </c>
       <c r="T10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="U10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -1335,41 +1335,41 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I11" t="n">
+        <v>6</v>
+      </c>
+      <c r="J11" t="n">
+        <v>5</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
         <v>4</v>
       </c>
-      <c r="J11" t="n">
+      <c r="P11" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q11" t="n">
         <v>3</v>
       </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>1</v>
-      </c>
-      <c r="N11" t="n">
-        <v>1</v>
-      </c>
-      <c r="O11" t="n">
+      <c r="R11" t="n">
         <v>3</v>
-      </c>
-      <c r="P11" t="n">
-        <v>11</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>2</v>
-      </c>
-      <c r="R11" t="n">
-        <v>2</v>
       </c>
       <c r="S11" t="n">
         <v>0</v>
@@ -1417,20 +1417,20 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="I12" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
@@ -1439,25 +1439,25 @@
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" t="n">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="Q12" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="R12" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="S12" t="n">
         <v>1</v>
       </c>
       <c r="T12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U12" t="n">
         <v>1</v>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1591,31 +1591,31 @@
         <v>3</v>
       </c>
       <c r="J14" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P14" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="Q14" t="n">
         <v>1</v>
       </c>
       <c r="R14" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -2058,17 +2058,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Sebastian Williams-Adams</t>
+          <t>Malique Ewin</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>AUB</t>
+          <t>ARK</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>VAN@AUB</t>
+          <t>ARK@LSU</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2080,7 +2080,7 @@
         <v>12</v>
       </c>
       <c r="I20" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J20" t="n">
         <v>6</v>
@@ -2095,31 +2095,31 @@
         <v>1</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20" t="n">
+        <v>3</v>
+      </c>
+      <c r="P20" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>3</v>
+      </c>
+      <c r="R20" t="n">
         <v>4</v>
       </c>
-      <c r="P20" t="n">
-        <v>37</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>4</v>
-      </c>
-      <c r="R20" t="n">
-        <v>9</v>
-      </c>
       <c r="S20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V20" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -2140,12 +2140,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>AK Okereke</t>
+          <t>Sebastian Williams-Adams</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>AUB</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2159,16 +2159,16 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I21" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J21" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L21" t="n">
         <v>0</v>
@@ -2177,25 +2177,25 @@
         <v>1</v>
       </c>
       <c r="N21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P21" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="Q21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R21" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="S21" t="n">
         <v>1</v>
       </c>
       <c r="T21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U21" t="n">
         <v>2</v>
@@ -2222,35 +2222,35 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Malique Ewin</t>
+          <t>AK Okereke</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>ARK</t>
+          <t>VAN</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ARK@LSU</t>
+          <t>VAN@AUB</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>8</v>
       </c>
       <c r="I22" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J22" t="n">
         <v>3</v>
       </c>
       <c r="K22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L22" t="n">
         <v>0</v>
@@ -2262,28 +2262,28 @@
         <v>1</v>
       </c>
       <c r="O22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P22" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="Q22" t="n">
         <v>2</v>
       </c>
       <c r="R22" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V22" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23">
@@ -2304,17 +2304,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Filip Jović</t>
+          <t>Robert Miller III</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>AUB</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>VAN@AUB</t>
+          <t>ARK@LSU</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2323,16 +2323,16 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I23" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J23" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" t="n">
         <v>0</v>
@@ -2341,13 +2341,13 @@
         <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23" t="n">
         <v>2</v>
       </c>
       <c r="P23" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="Q23" t="n">
         <v>2</v>
@@ -2362,10 +2362,10 @@
         <v>0</v>
       </c>
       <c r="U23" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="V23" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
@@ -2386,22 +2386,22 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Jalen Reece</t>
+          <t>Filip Jović</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>AUB</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>ARK@LSU</t>
+          <t>VAN@AUB</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -2411,10 +2411,10 @@
         <v>4</v>
       </c>
       <c r="J24" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K24" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
         <v>0</v>
@@ -2423,31 +2423,31 @@
         <v>0</v>
       </c>
       <c r="N24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24" t="n">
         <v>2</v>
       </c>
       <c r="P24" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="Q24" t="n">
         <v>2</v>
       </c>
       <c r="R24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S24" t="n">
         <v>0</v>
       </c>
       <c r="T24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U24" t="n">
         <v>0</v>
       </c>
       <c r="V24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -2468,17 +2468,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Chandler Bing</t>
+          <t>Mazi Mosley</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>VAN@AUB</t>
+          <t>ARK@LSU</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2487,10 +2487,10 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I25" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
@@ -2499,7 +2499,7 @@
         <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" t="n">
         <v>0</v>
@@ -2508,28 +2508,28 @@
         <v>1</v>
       </c>
       <c r="O25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P25" t="n">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="Q25" t="n">
+        <v>2</v>
+      </c>
+      <c r="R25" t="n">
         <v>3</v>
       </c>
-      <c r="R25" t="n">
-        <v>6</v>
-      </c>
       <c r="S25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" t="n">
         <v>2</v>
       </c>
       <c r="U25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V25" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -2550,32 +2550,32 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>PJ Carter</t>
+          <t>Chandler Bing</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>VAN</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>ARK@LSU</t>
+          <t>VAN@AUB</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H26" t="n">
         <v>4</v>
       </c>
       <c r="I26" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
         <v>0</v>
@@ -2593,25 +2593,25 @@
         <v>1</v>
       </c>
       <c r="P26" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="Q26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R26" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T26" t="n">
+        <v>2</v>
+      </c>
+      <c r="U26" t="n">
+        <v>2</v>
+      </c>
+      <c r="V26" t="n">
         <v>3</v>
-      </c>
-      <c r="U26" t="n">
-        <v>2</v>
-      </c>
-      <c r="V26" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -2632,7 +2632,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Rashad King</t>
+          <t>Jalen Reece</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2647,41 +2647,41 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H27" t="n">
+        <v>4</v>
+      </c>
+      <c r="I27" t="n">
+        <v>4</v>
+      </c>
+      <c r="J27" t="n">
+        <v>2</v>
+      </c>
+      <c r="K27" t="n">
+        <v>7</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>2</v>
+      </c>
+      <c r="O27" t="n">
         <v>3</v>
       </c>
-      <c r="I27" t="n">
-        <v>2</v>
-      </c>
-      <c r="J27" t="n">
-        <v>4</v>
-      </c>
-      <c r="K27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27" t="n">
-        <v>1</v>
-      </c>
       <c r="P27" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="Q27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R27" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="S27" t="n">
         <v>0</v>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Robert Miller III</t>
+          <t>Rashad King</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2729,53 +2729,53 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I28" t="n">
+        <v>2</v>
+      </c>
+      <c r="J28" t="n">
+        <v>5</v>
+      </c>
+      <c r="K28" t="n">
+        <v>2</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1</v>
+      </c>
+      <c r="P28" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>1</v>
+      </c>
+      <c r="R28" t="n">
         <v>7</v>
       </c>
-      <c r="J28" t="n">
-        <v>2</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" t="n">
-        <v>1</v>
-      </c>
-      <c r="O28" t="n">
-        <v>1</v>
-      </c>
-      <c r="P28" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>2</v>
-      </c>
-      <c r="R28" t="n">
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
         <v>4</v>
       </c>
-      <c r="S28" t="n">
-        <v>0</v>
-      </c>
-      <c r="T28" t="n">
-        <v>0</v>
-      </c>
       <c r="U28" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V28" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -2796,12 +2796,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Isaiah Sealy</t>
+          <t>Jaden Bobbett</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>ARK</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2811,20 +2811,20 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>16:11 - 2nd Half</t>
+          <t>Final</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" t="n">
         <v>0</v>
@@ -2836,16 +2836,16 @@
         <v>0</v>
       </c>
       <c r="O29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P29" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Q29" t="n">
         <v>0</v>
       </c>
       <c r="R29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S29" t="n">
         <v>0</v>
@@ -2854,10 +2854,10 @@
         <v>0</v>
       </c>
       <c r="U29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -2878,17 +2878,17 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Jayden Leverett</t>
+          <t>PJ Carter</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>VAN@AUB</t>
+          <t>ARK@LSU</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2897,49 +2897,49 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K30" t="n">
         <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" t="n">
         <v>0</v>
       </c>
       <c r="N30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P30" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="Q30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R30" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T30" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -2960,17 +2960,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Mike James</t>
+          <t>Isaiah Sealy</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>ARK</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>VAN@AUB</t>
+          <t>ARK@LSU</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2979,13 +2979,13 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31" t="n">
         <v>1</v>
@@ -3000,28 +3000,28 @@
         <v>1</v>
       </c>
       <c r="O31" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P31" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S31" t="n">
         <v>0</v>
       </c>
       <c r="T31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -3042,17 +3042,17 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Simon Walker</t>
+          <t>Jaden Karuletwa</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>AUB</t>
+          <t>ARK</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>VAN@AUB</t>
+          <t>ARK@LSU</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -3061,13 +3061,13 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" t="n">
         <v>0</v>
@@ -3082,7 +3082,7 @@
         <v>0</v>
       </c>
       <c r="O32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P32" t="n">
         <v>3</v>
@@ -3124,67 +3124,559 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
+          <t>Ayden Kelley</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>ARK</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>ARK@LSU</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Jayden Leverett</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>VAN</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>VAN@AUB</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Mike James</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>VAN</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>VAN@AUB</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>1</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" t="n">
+        <v>5</v>
+      </c>
+      <c r="P35" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>1</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>1</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Simon Walker</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>AUB</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>VAN@AUB</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="n">
+        <v>1</v>
+      </c>
+      <c r="P36" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="n">
+        <v>0</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0</v>
+      </c>
+      <c r="V36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Amere Brown</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>ARK</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>ARK@LSU</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
+        <v>1</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Elmir Džafić</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>ARK</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>ARK@LSU</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>1</v>
+      </c>
+      <c r="O38" t="n">
+        <v>1</v>
+      </c>
+      <c r="P38" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0</v>
+      </c>
+      <c r="V38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
           <t>Tyler Harris</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>VAN</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>VAN@AUB</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t>Final</t>
         </is>
       </c>
-      <c r="H33" t="n">
+      <c r="H39" t="n">
         <v>-1</v>
       </c>
-      <c r="I33" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" t="n">
-        <v>1</v>
-      </c>
-      <c r="N33" t="n">
-        <v>0</v>
-      </c>
-      <c r="O33" t="n">
-        <v>1</v>
-      </c>
-      <c r="P33" t="n">
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>1</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>1</v>
+      </c>
+      <c r="P39" t="n">
         <v>6</v>
       </c>
-      <c r="Q33" t="n">
-        <v>0</v>
-      </c>
-      <c r="R33" t="n">
-        <v>2</v>
-      </c>
-      <c r="S33" t="n">
-        <v>0</v>
-      </c>
-      <c r="T33" t="n">
-        <v>1</v>
-      </c>
-      <c r="U33" t="n">
-        <v>0</v>
-      </c>
-      <c r="V33" t="n">
+      <c r="Q39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="n">
+        <v>2</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="n">
+        <v>1</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
+      <c r="V39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3236,7 +3728,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C2" t="n">
         <v>3</v>
@@ -3262,7 +3754,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
@@ -3271,37 +3763,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Three Dawg Nite</t>
+          <t>Boozers Losers</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Hilton Heads</t>
+          <t>Three Dawg Nite</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Boozers Losers</t>
+          <t>Hilton Heads</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C7" t="n">
         <v>2</v>

</xml_diff>